<commit_message>
calorimetry : python : io csv
</commit_message>
<xml_diff>
--- a/output/calorimetry/map_6.xlsx
+++ b/output/calorimetry/map_6.xlsx
@@ -457,76 +457,76 @@
         <v>20782</v>
       </c>
       <c r="C2">
-        <v>15488</v>
+        <v>21255</v>
       </c>
       <c r="D2">
-        <v>10979</v>
+        <v>21740</v>
       </c>
       <c r="E2">
-        <v>7253</v>
+        <v>22237</v>
       </c>
       <c r="F2">
-        <v>4312</v>
+        <v>22746</v>
       </c>
       <c r="G2">
-        <v>2153</v>
+        <v>23268</v>
       </c>
       <c r="H2">
-        <v>777</v>
+        <v>23804</v>
       </c>
       <c r="I2">
-        <v>184</v>
+        <v>24352</v>
       </c>
       <c r="J2">
-        <v>371</v>
+        <v>24915</v>
       </c>
       <c r="K2">
-        <v>1340</v>
+        <v>25491</v>
       </c>
       <c r="L2">
-        <v>3088</v>
+        <v>26082</v>
       </c>
       <c r="M2">
-        <v>5614</v>
+        <v>26687</v>
       </c>
       <c r="N2">
-        <v>8917</v>
+        <v>27307</v>
       </c>
       <c r="O2">
-        <v>12996</v>
+        <v>27943</v>
       </c>
       <c r="P2">
-        <v>17849</v>
+        <v>28594</v>
       </c>
       <c r="Q2">
-        <v>23475</v>
+        <v>29262</v>
       </c>
       <c r="R2">
-        <v>29871</v>
+        <v>29946</v>
       </c>
       <c r="S2">
-        <v>37035</v>
+        <v>30646</v>
       </c>
       <c r="T2">
-        <v>44967</v>
+        <v>31364</v>
       </c>
       <c r="U2">
-        <v>53663</v>
+        <v>32099</v>
       </c>
       <c r="V2">
-        <v>63121</v>
+        <v>32853</v>
       </c>
       <c r="W2">
-        <v>73339</v>
+        <v>33625</v>
       </c>
       <c r="X2">
-        <v>84314</v>
+        <v>34415</v>
       </c>
       <c r="Y2">
-        <v>96044</v>
+        <v>35225</v>
       </c>
       <c r="Z2">
-        <v>108526</v>
+        <v>36055</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -534,79 +534,79 @@
         <v>3.45625</v>
       </c>
       <c r="B3">
-        <v>21255</v>
+        <v>15488</v>
       </c>
       <c r="C3">
         <v>15892</v>
       </c>
       <c r="D3">
-        <v>11314</v>
+        <v>16307</v>
       </c>
       <c r="E3">
-        <v>7521</v>
+        <v>16732</v>
       </c>
       <c r="F3">
-        <v>4513</v>
+        <v>17170</v>
       </c>
       <c r="G3">
-        <v>2288</v>
+        <v>17619</v>
       </c>
       <c r="H3">
-        <v>848</v>
+        <v>18080</v>
       </c>
       <c r="I3">
-        <v>191</v>
+        <v>18553</v>
       </c>
       <c r="J3">
-        <v>316</v>
+        <v>19040</v>
       </c>
       <c r="K3">
-        <v>1222</v>
+        <v>19539</v>
       </c>
       <c r="L3">
-        <v>2909</v>
+        <v>20052</v>
       </c>
       <c r="M3">
-        <v>5376</v>
+        <v>20578</v>
       </c>
       <c r="N3">
-        <v>8620</v>
+        <v>21118</v>
       </c>
       <c r="O3">
-        <v>12641</v>
+        <v>21673</v>
       </c>
       <c r="P3">
-        <v>17437</v>
+        <v>22242</v>
       </c>
       <c r="Q3">
-        <v>23006</v>
+        <v>22826</v>
       </c>
       <c r="R3">
-        <v>29347</v>
+        <v>23425</v>
       </c>
       <c r="S3">
-        <v>36458</v>
+        <v>24041</v>
       </c>
       <c r="T3">
-        <v>44336</v>
+        <v>24672</v>
       </c>
       <c r="U3">
-        <v>52979</v>
+        <v>25320</v>
       </c>
       <c r="V3">
-        <v>62386</v>
+        <v>25984</v>
       </c>
       <c r="W3">
-        <v>72554</v>
+        <v>26666</v>
       </c>
       <c r="X3">
-        <v>83479</v>
+        <v>27366</v>
       </c>
       <c r="Y3">
-        <v>95161</v>
+        <v>28083</v>
       </c>
       <c r="Z3">
-        <v>107595</v>
+        <v>28819</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -614,79 +614,79 @@
         <v>3.4625</v>
       </c>
       <c r="B4">
-        <v>21740</v>
+        <v>10979</v>
       </c>
       <c r="C4">
-        <v>16307</v>
+        <v>11314</v>
       </c>
       <c r="D4">
         <v>11659</v>
       </c>
       <c r="E4">
-        <v>7798</v>
+        <v>12015</v>
       </c>
       <c r="F4">
-        <v>4722</v>
+        <v>12381</v>
       </c>
       <c r="G4">
-        <v>2431</v>
+        <v>12758</v>
       </c>
       <c r="H4">
-        <v>925</v>
+        <v>13146</v>
       </c>
       <c r="I4">
-        <v>204</v>
+        <v>13545</v>
       </c>
       <c r="J4">
-        <v>265</v>
+        <v>13957</v>
       </c>
       <c r="K4">
-        <v>1109</v>
+        <v>14380</v>
       </c>
       <c r="L4">
-        <v>2735</v>
+        <v>14816</v>
       </c>
       <c r="M4">
-        <v>5140</v>
+        <v>15264</v>
       </c>
       <c r="N4">
-        <v>8325</v>
+        <v>15725</v>
       </c>
       <c r="O4">
-        <v>12287</v>
+        <v>16200</v>
       </c>
       <c r="P4">
-        <v>17025</v>
+        <v>16688</v>
       </c>
       <c r="Q4">
-        <v>22538</v>
+        <v>17190</v>
       </c>
       <c r="R4">
-        <v>28822</v>
+        <v>17706</v>
       </c>
       <c r="S4">
-        <v>35878</v>
+        <v>18237</v>
       </c>
       <c r="T4">
-        <v>43702</v>
+        <v>18783</v>
       </c>
       <c r="U4">
-        <v>52293</v>
+        <v>19344</v>
       </c>
       <c r="V4">
-        <v>61647</v>
+        <v>19921</v>
       </c>
       <c r="W4">
-        <v>71764</v>
+        <v>20515</v>
       </c>
       <c r="X4">
-        <v>82639</v>
+        <v>21124</v>
       </c>
       <c r="Y4">
-        <v>94271</v>
+        <v>21751</v>
       </c>
       <c r="Z4">
-        <v>106657</v>
+        <v>22395</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -694,79 +694,79 @@
         <v>3.46875</v>
       </c>
       <c r="B5">
-        <v>22237</v>
+        <v>7253</v>
       </c>
       <c r="C5">
-        <v>16732</v>
+        <v>7521</v>
       </c>
       <c r="D5">
-        <v>12015</v>
+        <v>7798</v>
       </c>
       <c r="E5">
         <v>8084</v>
       </c>
       <c r="F5">
-        <v>4940</v>
+        <v>8380</v>
       </c>
       <c r="G5">
-        <v>2582</v>
+        <v>8686</v>
       </c>
       <c r="H5">
-        <v>1010</v>
+        <v>9002</v>
       </c>
       <c r="I5">
-        <v>222</v>
+        <v>9328</v>
       </c>
       <c r="J5">
-        <v>220</v>
+        <v>9666</v>
       </c>
       <c r="K5">
-        <v>1000</v>
+        <v>10014</v>
       </c>
       <c r="L5">
-        <v>2563</v>
+        <v>10374</v>
       </c>
       <c r="M5">
-        <v>4907</v>
+        <v>10745</v>
       </c>
       <c r="N5">
-        <v>8031</v>
+        <v>11129</v>
       </c>
       <c r="O5">
-        <v>11934</v>
+        <v>11524</v>
       </c>
       <c r="P5">
-        <v>16614</v>
+        <v>11932</v>
       </c>
       <c r="Q5">
-        <v>22068</v>
+        <v>12353</v>
       </c>
       <c r="R5">
-        <v>28297</v>
+        <v>12788</v>
       </c>
       <c r="S5">
-        <v>35296</v>
+        <v>13236</v>
       </c>
       <c r="T5">
-        <v>43066</v>
+        <v>13697</v>
       </c>
       <c r="U5">
-        <v>51603</v>
+        <v>14173</v>
       </c>
       <c r="V5">
-        <v>60904</v>
+        <v>14664</v>
       </c>
       <c r="W5">
-        <v>70969</v>
+        <v>15170</v>
       </c>
       <c r="X5">
-        <v>81793</v>
+        <v>15691</v>
       </c>
       <c r="Y5">
-        <v>93375</v>
+        <v>16228</v>
       </c>
       <c r="Z5">
-        <v>105712</v>
+        <v>16781</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -774,79 +774,79 @@
         <v>3.475</v>
       </c>
       <c r="B6">
-        <v>22746</v>
+        <v>4312</v>
       </c>
       <c r="C6">
-        <v>17170</v>
+        <v>4513</v>
       </c>
       <c r="D6">
-        <v>12381</v>
+        <v>4722</v>
       </c>
       <c r="E6">
-        <v>8380</v>
+        <v>4940</v>
       </c>
       <c r="F6">
         <v>5166</v>
       </c>
       <c r="G6">
-        <v>2740</v>
+        <v>5402</v>
       </c>
       <c r="H6">
-        <v>1101</v>
+        <v>5647</v>
       </c>
       <c r="I6">
-        <v>247</v>
+        <v>5902</v>
       </c>
       <c r="J6">
-        <v>179</v>
+        <v>6166</v>
       </c>
       <c r="K6">
-        <v>896</v>
+        <v>6441</v>
       </c>
       <c r="L6">
-        <v>2395</v>
+        <v>6726</v>
       </c>
       <c r="M6">
-        <v>4677</v>
+        <v>7021</v>
       </c>
       <c r="N6">
-        <v>7740</v>
+        <v>7328</v>
       </c>
       <c r="O6">
-        <v>11582</v>
+        <v>7646</v>
       </c>
       <c r="P6">
-        <v>16202</v>
+        <v>7975</v>
       </c>
       <c r="Q6">
-        <v>21599</v>
+        <v>8316</v>
       </c>
       <c r="R6">
-        <v>27770</v>
+        <v>8670</v>
       </c>
       <c r="S6">
-        <v>34713</v>
+        <v>9036</v>
       </c>
       <c r="T6">
-        <v>42427</v>
+        <v>9415</v>
       </c>
       <c r="U6">
-        <v>50909</v>
+        <v>9807</v>
       </c>
       <c r="V6">
-        <v>60157</v>
+        <v>10212</v>
       </c>
       <c r="W6">
-        <v>70169</v>
+        <v>10631</v>
       </c>
       <c r="X6">
-        <v>80942</v>
+        <v>11065</v>
       </c>
       <c r="Y6">
-        <v>92473</v>
+        <v>11514</v>
       </c>
       <c r="Z6">
-        <v>104760</v>
+        <v>11977</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -854,79 +854,79 @@
         <v>3.48125</v>
       </c>
       <c r="B7">
-        <v>23268</v>
+        <v>2153</v>
       </c>
       <c r="C7">
-        <v>17619</v>
+        <v>2288</v>
       </c>
       <c r="D7">
-        <v>12758</v>
+        <v>2431</v>
       </c>
       <c r="E7">
-        <v>8686</v>
+        <v>2582</v>
       </c>
       <c r="F7">
-        <v>5402</v>
+        <v>2740</v>
       </c>
       <c r="G7">
         <v>2907</v>
       </c>
       <c r="H7">
-        <v>1199</v>
+        <v>3082</v>
       </c>
       <c r="I7">
-        <v>279</v>
+        <v>3266</v>
       </c>
       <c r="J7">
-        <v>145</v>
+        <v>3458</v>
       </c>
       <c r="K7">
-        <v>796</v>
+        <v>3660</v>
       </c>
       <c r="L7">
-        <v>2231</v>
+        <v>3871</v>
       </c>
       <c r="M7">
-        <v>4450</v>
+        <v>4092</v>
       </c>
       <c r="N7">
-        <v>7451</v>
+        <v>4323</v>
       </c>
       <c r="O7">
-        <v>11232</v>
+        <v>4564</v>
       </c>
       <c r="P7">
-        <v>15792</v>
+        <v>4816</v>
       </c>
       <c r="Q7">
-        <v>21129</v>
+        <v>5078</v>
       </c>
       <c r="R7">
-        <v>27242</v>
+        <v>5352</v>
       </c>
       <c r="S7">
-        <v>34128</v>
+        <v>5637</v>
       </c>
       <c r="T7">
-        <v>41786</v>
+        <v>5934</v>
       </c>
       <c r="U7">
-        <v>50213</v>
+        <v>6243</v>
       </c>
       <c r="V7">
-        <v>59406</v>
+        <v>6565</v>
       </c>
       <c r="W7">
-        <v>69365</v>
+        <v>6899</v>
       </c>
       <c r="X7">
-        <v>80086</v>
+        <v>7247</v>
       </c>
       <c r="Y7">
-        <v>91565</v>
+        <v>7608</v>
       </c>
       <c r="Z7">
-        <v>103802</v>
+        <v>7983</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -934,79 +934,79 @@
         <v>3.4875</v>
       </c>
       <c r="B8">
-        <v>23804</v>
+        <v>777</v>
       </c>
       <c r="C8">
-        <v>18080</v>
+        <v>848</v>
       </c>
       <c r="D8">
-        <v>13146</v>
+        <v>925</v>
       </c>
       <c r="E8">
-        <v>9002</v>
+        <v>1010</v>
       </c>
       <c r="F8">
-        <v>5647</v>
+        <v>1101</v>
       </c>
       <c r="G8">
-        <v>3082</v>
+        <v>1199</v>
       </c>
       <c r="H8">
         <v>1305</v>
       </c>
       <c r="I8">
-        <v>317</v>
+        <v>1419</v>
       </c>
       <c r="J8">
-        <v>116</v>
+        <v>1541</v>
       </c>
       <c r="K8">
-        <v>701</v>
+        <v>1671</v>
       </c>
       <c r="L8">
-        <v>2072</v>
+        <v>1809</v>
       </c>
       <c r="M8">
-        <v>4226</v>
+        <v>1957</v>
       </c>
       <c r="N8">
-        <v>7164</v>
+        <v>2113</v>
       </c>
       <c r="O8">
-        <v>10883</v>
+        <v>2278</v>
       </c>
       <c r="P8">
-        <v>15382</v>
+        <v>2454</v>
       </c>
       <c r="Q8">
-        <v>20659</v>
+        <v>2638</v>
       </c>
       <c r="R8">
-        <v>26713</v>
+        <v>2834</v>
       </c>
       <c r="S8">
-        <v>33541</v>
+        <v>3039</v>
       </c>
       <c r="T8">
-        <v>41142</v>
+        <v>3256</v>
       </c>
       <c r="U8">
-        <v>49513</v>
+        <v>3483</v>
       </c>
       <c r="V8">
-        <v>58652</v>
+        <v>3722</v>
       </c>
       <c r="W8">
-        <v>68556</v>
+        <v>3972</v>
       </c>
       <c r="X8">
-        <v>79224</v>
+        <v>4235</v>
       </c>
       <c r="Y8">
-        <v>90652</v>
+        <v>4510</v>
       </c>
       <c r="Z8">
-        <v>102837</v>
+        <v>4798</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1014,79 +1014,79 @@
         <v>3.49375</v>
       </c>
       <c r="B9">
-        <v>24352</v>
+        <v>184</v>
       </c>
       <c r="C9">
-        <v>18553</v>
+        <v>191</v>
       </c>
       <c r="D9">
-        <v>13545</v>
+        <v>204</v>
       </c>
       <c r="E9">
-        <v>9328</v>
+        <v>222</v>
       </c>
       <c r="F9">
-        <v>5902</v>
+        <v>247</v>
       </c>
       <c r="G9">
-        <v>3266</v>
+        <v>279</v>
       </c>
       <c r="H9">
-        <v>1419</v>
+        <v>317</v>
       </c>
       <c r="I9">
         <v>362</v>
       </c>
       <c r="J9">
-        <v>93</v>
+        <v>414</v>
       </c>
       <c r="K9">
-        <v>611</v>
+        <v>473</v>
       </c>
       <c r="L9">
-        <v>1916</v>
+        <v>540</v>
       </c>
       <c r="M9">
-        <v>4006</v>
+        <v>615</v>
       </c>
       <c r="N9">
-        <v>6880</v>
+        <v>697</v>
       </c>
       <c r="O9">
-        <v>10536</v>
+        <v>788</v>
       </c>
       <c r="P9">
-        <v>14973</v>
+        <v>888</v>
       </c>
       <c r="Q9">
-        <v>20190</v>
+        <v>997</v>
       </c>
       <c r="R9">
-        <v>26184</v>
+        <v>1114</v>
       </c>
       <c r="S9">
-        <v>32953</v>
+        <v>1241</v>
       </c>
       <c r="T9">
-        <v>40496</v>
+        <v>1378</v>
       </c>
       <c r="U9">
-        <v>48810</v>
+        <v>1525</v>
       </c>
       <c r="V9">
-        <v>57893</v>
+        <v>1682</v>
       </c>
       <c r="W9">
-        <v>67743</v>
+        <v>1850</v>
       </c>
       <c r="X9">
-        <v>78357</v>
+        <v>2029</v>
       </c>
       <c r="Y9">
-        <v>89732</v>
+        <v>2220</v>
       </c>
       <c r="Z9">
-        <v>101866</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -1094,79 +1094,79 @@
         <v>3.5</v>
       </c>
       <c r="B10">
-        <v>24915</v>
+        <v>371</v>
       </c>
       <c r="C10">
-        <v>19040</v>
+        <v>316</v>
       </c>
       <c r="D10">
-        <v>13957</v>
+        <v>265</v>
       </c>
       <c r="E10">
-        <v>9666</v>
+        <v>220</v>
       </c>
       <c r="F10">
-        <v>6166</v>
+        <v>179</v>
       </c>
       <c r="G10">
-        <v>3458</v>
+        <v>145</v>
       </c>
       <c r="H10">
-        <v>1541</v>
+        <v>116</v>
       </c>
       <c r="I10">
-        <v>414</v>
+        <v>93</v>
       </c>
       <c r="J10">
         <v>76</v>
       </c>
       <c r="K10">
-        <v>527</v>
+        <v>66</v>
       </c>
       <c r="L10">
-        <v>1765</v>
+        <v>62</v>
       </c>
       <c r="M10">
-        <v>3789</v>
+        <v>65</v>
       </c>
       <c r="N10">
-        <v>6598</v>
+        <v>75</v>
       </c>
       <c r="O10">
-        <v>10191</v>
+        <v>93</v>
       </c>
       <c r="P10">
-        <v>14566</v>
+        <v>118</v>
       </c>
       <c r="Q10">
-        <v>19721</v>
+        <v>152</v>
       </c>
       <c r="R10">
-        <v>25654</v>
+        <v>193</v>
       </c>
       <c r="S10">
-        <v>32364</v>
+        <v>243</v>
       </c>
       <c r="T10">
-        <v>39848</v>
+        <v>301</v>
       </c>
       <c r="U10">
-        <v>48105</v>
+        <v>369</v>
       </c>
       <c r="V10">
-        <v>57132</v>
+        <v>446</v>
       </c>
       <c r="W10">
-        <v>66926</v>
+        <v>532</v>
       </c>
       <c r="X10">
-        <v>77485</v>
+        <v>629</v>
       </c>
       <c r="Y10">
-        <v>88806</v>
+        <v>736</v>
       </c>
       <c r="Z10">
-        <v>100888</v>
+        <v>853</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -1174,79 +1174,79 @@
         <v>3.50625</v>
       </c>
       <c r="B11">
-        <v>25491</v>
+        <v>1340</v>
       </c>
       <c r="C11">
-        <v>19539</v>
+        <v>1222</v>
       </c>
       <c r="D11">
-        <v>14380</v>
+        <v>1109</v>
       </c>
       <c r="E11">
-        <v>10014</v>
+        <v>1000</v>
       </c>
       <c r="F11">
-        <v>6441</v>
+        <v>896</v>
       </c>
       <c r="G11">
-        <v>3660</v>
+        <v>796</v>
       </c>
       <c r="H11">
-        <v>1671</v>
+        <v>701</v>
       </c>
       <c r="I11">
-        <v>473</v>
+        <v>611</v>
       </c>
       <c r="J11">
-        <v>66</v>
+        <v>527</v>
       </c>
       <c r="K11">
         <v>448</v>
       </c>
       <c r="L11">
-        <v>1618</v>
+        <v>374</v>
       </c>
       <c r="M11">
-        <v>3576</v>
+        <v>307</v>
       </c>
       <c r="N11">
-        <v>6320</v>
+        <v>246</v>
       </c>
       <c r="O11">
-        <v>9848</v>
+        <v>191</v>
       </c>
       <c r="P11">
-        <v>14159</v>
+        <v>144</v>
       </c>
       <c r="Q11">
-        <v>19252</v>
+        <v>103</v>
       </c>
       <c r="R11">
-        <v>25124</v>
+        <v>69</v>
       </c>
       <c r="S11">
-        <v>31773</v>
+        <v>42</v>
       </c>
       <c r="T11">
-        <v>39198</v>
+        <v>24</v>
       </c>
       <c r="U11">
-        <v>47397</v>
+        <v>13</v>
       </c>
       <c r="V11">
-        <v>56366</v>
+        <v>11</v>
       </c>
       <c r="W11">
-        <v>66104</v>
+        <v>18</v>
       </c>
       <c r="X11">
-        <v>76608</v>
+        <v>33</v>
       </c>
       <c r="Y11">
-        <v>87875</v>
+        <v>57</v>
       </c>
       <c r="Z11">
-        <v>99903</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -1254,79 +1254,79 @@
         <v>3.5125</v>
       </c>
       <c r="B12">
-        <v>26082</v>
+        <v>3088</v>
       </c>
       <c r="C12">
-        <v>20052</v>
+        <v>2909</v>
       </c>
       <c r="D12">
-        <v>14816</v>
+        <v>2735</v>
       </c>
       <c r="E12">
-        <v>10374</v>
+        <v>2563</v>
       </c>
       <c r="F12">
-        <v>6726</v>
+        <v>2395</v>
       </c>
       <c r="G12">
-        <v>3871</v>
+        <v>2231</v>
       </c>
       <c r="H12">
-        <v>1809</v>
+        <v>2072</v>
       </c>
       <c r="I12">
-        <v>540</v>
+        <v>1916</v>
       </c>
       <c r="J12">
-        <v>62</v>
+        <v>1765</v>
       </c>
       <c r="K12">
-        <v>374</v>
+        <v>1618</v>
       </c>
       <c r="L12">
         <v>1476</v>
       </c>
       <c r="M12">
-        <v>3367</v>
+        <v>1340</v>
       </c>
       <c r="N12">
-        <v>6044</v>
+        <v>1208</v>
       </c>
       <c r="O12">
-        <v>9507</v>
+        <v>1083</v>
       </c>
       <c r="P12">
-        <v>13754</v>
+        <v>963</v>
       </c>
       <c r="Q12">
-        <v>18783</v>
+        <v>849</v>
       </c>
       <c r="R12">
-        <v>24593</v>
+        <v>741</v>
       </c>
       <c r="S12">
-        <v>31182</v>
+        <v>639</v>
       </c>
       <c r="T12">
-        <v>38547</v>
+        <v>545</v>
       </c>
       <c r="U12">
-        <v>46686</v>
+        <v>457</v>
       </c>
       <c r="V12">
-        <v>55597</v>
+        <v>377</v>
       </c>
       <c r="W12">
-        <v>65278</v>
+        <v>305</v>
       </c>
       <c r="X12">
-        <v>75726</v>
+        <v>240</v>
       </c>
       <c r="Y12">
-        <v>86938</v>
+        <v>183</v>
       </c>
       <c r="Z12">
-        <v>98912</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -1334,79 +1334,79 @@
         <v>3.51875</v>
       </c>
       <c r="B13">
-        <v>26687</v>
+        <v>5614</v>
       </c>
       <c r="C13">
-        <v>20578</v>
+        <v>5376</v>
       </c>
       <c r="D13">
-        <v>15264</v>
+        <v>5140</v>
       </c>
       <c r="E13">
-        <v>10745</v>
+        <v>4907</v>
       </c>
       <c r="F13">
-        <v>7021</v>
+        <v>4677</v>
       </c>
       <c r="G13">
-        <v>4092</v>
+        <v>4450</v>
       </c>
       <c r="H13">
-        <v>1957</v>
+        <v>4226</v>
       </c>
       <c r="I13">
-        <v>615</v>
+        <v>4006</v>
       </c>
       <c r="J13">
-        <v>65</v>
+        <v>3789</v>
       </c>
       <c r="K13">
-        <v>307</v>
+        <v>3576</v>
       </c>
       <c r="L13">
-        <v>1340</v>
+        <v>3367</v>
       </c>
       <c r="M13">
         <v>3162</v>
       </c>
       <c r="N13">
-        <v>5772</v>
+        <v>2961</v>
       </c>
       <c r="O13">
-        <v>9169</v>
+        <v>2765</v>
       </c>
       <c r="P13">
-        <v>13351</v>
+        <v>2574</v>
       </c>
       <c r="Q13">
-        <v>18316</v>
+        <v>2388</v>
       </c>
       <c r="R13">
-        <v>24063</v>
+        <v>2208</v>
       </c>
       <c r="S13">
-        <v>30589</v>
+        <v>2032</v>
       </c>
       <c r="T13">
-        <v>37893</v>
+        <v>1863</v>
       </c>
       <c r="U13">
-        <v>45973</v>
+        <v>1700</v>
       </c>
       <c r="V13">
-        <v>54825</v>
+        <v>1543</v>
       </c>
       <c r="W13">
-        <v>64448</v>
+        <v>1392</v>
       </c>
       <c r="X13">
-        <v>74839</v>
+        <v>1249</v>
       </c>
       <c r="Y13">
-        <v>85996</v>
+        <v>1112</v>
       </c>
       <c r="Z13">
-        <v>97915</v>
+        <v>983</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -1414,79 +1414,79 @@
         <v>3.525</v>
       </c>
       <c r="B14">
-        <v>27307</v>
+        <v>8917</v>
       </c>
       <c r="C14">
-        <v>21118</v>
+        <v>8620</v>
       </c>
       <c r="D14">
-        <v>15725</v>
+        <v>8325</v>
       </c>
       <c r="E14">
-        <v>11129</v>
+        <v>8031</v>
       </c>
       <c r="F14">
-        <v>7328</v>
+        <v>7740</v>
       </c>
       <c r="G14">
-        <v>4323</v>
+        <v>7451</v>
       </c>
       <c r="H14">
-        <v>2113</v>
+        <v>7164</v>
       </c>
       <c r="I14">
-        <v>697</v>
+        <v>6880</v>
       </c>
       <c r="J14">
-        <v>75</v>
+        <v>6598</v>
       </c>
       <c r="K14">
-        <v>246</v>
+        <v>6320</v>
       </c>
       <c r="L14">
-        <v>1208</v>
+        <v>6044</v>
       </c>
       <c r="M14">
-        <v>2961</v>
+        <v>5772</v>
       </c>
       <c r="N14">
         <v>5503</v>
       </c>
       <c r="O14">
-        <v>8833</v>
+        <v>5238</v>
       </c>
       <c r="P14">
-        <v>12949</v>
+        <v>4977</v>
       </c>
       <c r="Q14">
-        <v>17849</v>
+        <v>4721</v>
       </c>
       <c r="R14">
-        <v>23532</v>
+        <v>4468</v>
       </c>
       <c r="S14">
-        <v>29996</v>
+        <v>4220</v>
       </c>
       <c r="T14">
-        <v>37238</v>
+        <v>3977</v>
       </c>
       <c r="U14">
-        <v>45257</v>
+        <v>3739</v>
       </c>
       <c r="V14">
-        <v>54050</v>
+        <v>3507</v>
       </c>
       <c r="W14">
-        <v>63614</v>
+        <v>3280</v>
       </c>
       <c r="X14">
-        <v>73948</v>
+        <v>3058</v>
       </c>
       <c r="Y14">
-        <v>85048</v>
+        <v>2843</v>
       </c>
       <c r="Z14">
-        <v>96912</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -1494,79 +1494,79 @@
         <v>3.53125</v>
       </c>
       <c r="B15">
-        <v>27943</v>
+        <v>12996</v>
       </c>
       <c r="C15">
-        <v>21673</v>
+        <v>12641</v>
       </c>
       <c r="D15">
-        <v>16200</v>
+        <v>12287</v>
       </c>
       <c r="E15">
-        <v>11524</v>
+        <v>11934</v>
       </c>
       <c r="F15">
-        <v>7646</v>
+        <v>11582</v>
       </c>
       <c r="G15">
-        <v>4564</v>
+        <v>11232</v>
       </c>
       <c r="H15">
-        <v>2278</v>
+        <v>10883</v>
       </c>
       <c r="I15">
-        <v>788</v>
+        <v>10536</v>
       </c>
       <c r="J15">
-        <v>93</v>
+        <v>10191</v>
       </c>
       <c r="K15">
-        <v>191</v>
+        <v>9848</v>
       </c>
       <c r="L15">
-        <v>1083</v>
+        <v>9507</v>
       </c>
       <c r="M15">
-        <v>2765</v>
+        <v>9169</v>
       </c>
       <c r="N15">
-        <v>5238</v>
+        <v>8833</v>
       </c>
       <c r="O15">
         <v>8500</v>
       </c>
       <c r="P15">
-        <v>12549</v>
+        <v>8170</v>
       </c>
       <c r="Q15">
-        <v>17384</v>
+        <v>7844</v>
       </c>
       <c r="R15">
-        <v>23002</v>
+        <v>7521</v>
       </c>
       <c r="S15">
-        <v>29402</v>
+        <v>7201</v>
       </c>
       <c r="T15">
-        <v>36582</v>
+        <v>6886</v>
       </c>
       <c r="U15">
-        <v>44539</v>
+        <v>6574</v>
       </c>
       <c r="V15">
-        <v>53271</v>
+        <v>6267</v>
       </c>
       <c r="W15">
-        <v>62776</v>
+        <v>5965</v>
       </c>
       <c r="X15">
-        <v>73052</v>
+        <v>5667</v>
       </c>
       <c r="Y15">
-        <v>84094</v>
+        <v>5375</v>
       </c>
       <c r="Z15">
-        <v>95902</v>
+        <v>5088</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -1574,79 +1574,79 @@
         <v>3.5375</v>
       </c>
       <c r="B16">
-        <v>28594</v>
+        <v>17849</v>
       </c>
       <c r="C16">
-        <v>22242</v>
+        <v>17437</v>
       </c>
       <c r="D16">
-        <v>16688</v>
+        <v>17025</v>
       </c>
       <c r="E16">
-        <v>11932</v>
+        <v>16614</v>
       </c>
       <c r="F16">
-        <v>7975</v>
+        <v>16202</v>
       </c>
       <c r="G16">
-        <v>4816</v>
+        <v>15792</v>
       </c>
       <c r="H16">
-        <v>2454</v>
+        <v>15382</v>
       </c>
       <c r="I16">
-        <v>888</v>
+        <v>14973</v>
       </c>
       <c r="J16">
-        <v>118</v>
+        <v>14566</v>
       </c>
       <c r="K16">
-        <v>144</v>
+        <v>14159</v>
       </c>
       <c r="L16">
-        <v>963</v>
+        <v>13754</v>
       </c>
       <c r="M16">
-        <v>2574</v>
+        <v>13351</v>
       </c>
       <c r="N16">
-        <v>4977</v>
+        <v>12949</v>
       </c>
       <c r="O16">
-        <v>8170</v>
+        <v>12549</v>
       </c>
       <c r="P16">
         <v>12152</v>
       </c>
       <c r="Q16">
-        <v>16920</v>
+        <v>11756</v>
       </c>
       <c r="R16">
-        <v>22472</v>
+        <v>11364</v>
       </c>
       <c r="S16">
-        <v>28808</v>
+        <v>10974</v>
       </c>
       <c r="T16">
-        <v>35924</v>
+        <v>10587</v>
       </c>
       <c r="U16">
-        <v>43819</v>
+        <v>10203</v>
       </c>
       <c r="V16">
-        <v>52490</v>
+        <v>9823</v>
       </c>
       <c r="W16">
-        <v>61935</v>
+        <v>9446</v>
       </c>
       <c r="X16">
-        <v>72151</v>
+        <v>9073</v>
       </c>
       <c r="Y16">
-        <v>83136</v>
+        <v>8705</v>
       </c>
       <c r="Z16">
-        <v>94887</v>
+        <v>8341</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -1654,79 +1654,79 @@
         <v>3.54375</v>
       </c>
       <c r="B17">
-        <v>29262</v>
+        <v>23475</v>
       </c>
       <c r="C17">
-        <v>22826</v>
+        <v>23006</v>
       </c>
       <c r="D17">
-        <v>17190</v>
+        <v>22538</v>
       </c>
       <c r="E17">
-        <v>12353</v>
+        <v>22068</v>
       </c>
       <c r="F17">
-        <v>8316</v>
+        <v>21599</v>
       </c>
       <c r="G17">
-        <v>5078</v>
+        <v>21129</v>
       </c>
       <c r="H17">
-        <v>2638</v>
+        <v>20659</v>
       </c>
       <c r="I17">
-        <v>997</v>
+        <v>20190</v>
       </c>
       <c r="J17">
-        <v>152</v>
+        <v>19721</v>
       </c>
       <c r="K17">
-        <v>103</v>
+        <v>19252</v>
       </c>
       <c r="L17">
-        <v>849</v>
+        <v>18783</v>
       </c>
       <c r="M17">
-        <v>2388</v>
+        <v>18316</v>
       </c>
       <c r="N17">
-        <v>4721</v>
+        <v>17849</v>
       </c>
       <c r="O17">
-        <v>7844</v>
+        <v>17384</v>
       </c>
       <c r="P17">
-        <v>11756</v>
+        <v>16920</v>
       </c>
       <c r="Q17">
         <v>16457</v>
       </c>
       <c r="R17">
-        <v>21943</v>
+        <v>15996</v>
       </c>
       <c r="S17">
-        <v>28213</v>
+        <v>15537</v>
       </c>
       <c r="T17">
-        <v>35265</v>
+        <v>15079</v>
       </c>
       <c r="U17">
-        <v>43097</v>
+        <v>14624</v>
       </c>
       <c r="V17">
-        <v>51706</v>
+        <v>14172</v>
       </c>
       <c r="W17">
-        <v>61090</v>
+        <v>13722</v>
       </c>
       <c r="X17">
-        <v>71246</v>
+        <v>13275</v>
       </c>
       <c r="Y17">
-        <v>82172</v>
+        <v>12832</v>
       </c>
       <c r="Z17">
-        <v>93865</v>
+        <v>12392</v>
       </c>
     </row>
     <row r="18" spans="1:26">
@@ -1734,79 +1734,79 @@
         <v>3.55</v>
       </c>
       <c r="B18">
-        <v>29946</v>
+        <v>29871</v>
       </c>
       <c r="C18">
-        <v>23425</v>
+        <v>29347</v>
       </c>
       <c r="D18">
-        <v>17706</v>
+        <v>28822</v>
       </c>
       <c r="E18">
-        <v>12788</v>
+        <v>28297</v>
       </c>
       <c r="F18">
-        <v>8670</v>
+        <v>27770</v>
       </c>
       <c r="G18">
-        <v>5352</v>
+        <v>27242</v>
       </c>
       <c r="H18">
-        <v>2834</v>
+        <v>26713</v>
       </c>
       <c r="I18">
-        <v>1114</v>
+        <v>26184</v>
       </c>
       <c r="J18">
-        <v>193</v>
+        <v>25654</v>
       </c>
       <c r="K18">
-        <v>69</v>
+        <v>25124</v>
       </c>
       <c r="L18">
-        <v>741</v>
+        <v>24593</v>
       </c>
       <c r="M18">
-        <v>2208</v>
+        <v>24063</v>
       </c>
       <c r="N18">
-        <v>4468</v>
+        <v>23532</v>
       </c>
       <c r="O18">
-        <v>7521</v>
+        <v>23002</v>
       </c>
       <c r="P18">
-        <v>11364</v>
+        <v>22472</v>
       </c>
       <c r="Q18">
-        <v>15996</v>
+        <v>21943</v>
       </c>
       <c r="R18">
         <v>21415</v>
       </c>
       <c r="S18">
-        <v>27619</v>
+        <v>20887</v>
       </c>
       <c r="T18">
-        <v>34606</v>
+        <v>20361</v>
       </c>
       <c r="U18">
-        <v>42373</v>
+        <v>19836</v>
       </c>
       <c r="V18">
-        <v>50919</v>
+        <v>19313</v>
       </c>
       <c r="W18">
-        <v>60241</v>
+        <v>18791</v>
       </c>
       <c r="X18">
-        <v>70337</v>
+        <v>18271</v>
       </c>
       <c r="Y18">
-        <v>81203</v>
+        <v>17754</v>
       </c>
       <c r="Z18">
-        <v>92838</v>
+        <v>17239</v>
       </c>
     </row>
     <row r="19" spans="1:26">
@@ -1814,79 +1814,79 @@
         <v>3.55625</v>
       </c>
       <c r="B19">
-        <v>30646</v>
+        <v>37035</v>
       </c>
       <c r="C19">
-        <v>24041</v>
+        <v>36458</v>
       </c>
       <c r="D19">
-        <v>18237</v>
+        <v>35878</v>
       </c>
       <c r="E19">
-        <v>13236</v>
+        <v>35296</v>
       </c>
       <c r="F19">
-        <v>9036</v>
+        <v>34713</v>
       </c>
       <c r="G19">
-        <v>5637</v>
+        <v>34128</v>
       </c>
       <c r="H19">
-        <v>3039</v>
+        <v>33541</v>
       </c>
       <c r="I19">
-        <v>1241</v>
+        <v>32953</v>
       </c>
       <c r="J19">
-        <v>243</v>
+        <v>32364</v>
       </c>
       <c r="K19">
-        <v>42</v>
+        <v>31773</v>
       </c>
       <c r="L19">
-        <v>639</v>
+        <v>31182</v>
       </c>
       <c r="M19">
-        <v>2032</v>
+        <v>30589</v>
       </c>
       <c r="N19">
-        <v>4220</v>
+        <v>29996</v>
       </c>
       <c r="O19">
-        <v>7201</v>
+        <v>29402</v>
       </c>
       <c r="P19">
-        <v>10974</v>
+        <v>28808</v>
       </c>
       <c r="Q19">
-        <v>15537</v>
+        <v>28213</v>
       </c>
       <c r="R19">
-        <v>20887</v>
+        <v>27619</v>
       </c>
       <c r="S19">
         <v>27024</v>
       </c>
       <c r="T19">
-        <v>33945</v>
+        <v>26430</v>
       </c>
       <c r="U19">
-        <v>41648</v>
+        <v>25836</v>
       </c>
       <c r="V19">
-        <v>50130</v>
+        <v>25243</v>
       </c>
       <c r="W19">
-        <v>59390</v>
+        <v>24651</v>
       </c>
       <c r="X19">
-        <v>69424</v>
+        <v>24059</v>
       </c>
       <c r="Y19">
-        <v>80230</v>
+        <v>23469</v>
       </c>
       <c r="Z19">
-        <v>91805</v>
+        <v>22881</v>
       </c>
     </row>
     <row r="20" spans="1:26">
@@ -1894,79 +1894,79 @@
         <v>3.5625</v>
       </c>
       <c r="B20">
-        <v>31364</v>
+        <v>44967</v>
       </c>
       <c r="C20">
-        <v>24672</v>
+        <v>44336</v>
       </c>
       <c r="D20">
-        <v>18783</v>
+        <v>43702</v>
       </c>
       <c r="E20">
-        <v>13697</v>
+        <v>43066</v>
       </c>
       <c r="F20">
-        <v>9415</v>
+        <v>42427</v>
       </c>
       <c r="G20">
-        <v>5934</v>
+        <v>41786</v>
       </c>
       <c r="H20">
-        <v>3256</v>
+        <v>41142</v>
       </c>
       <c r="I20">
-        <v>1378</v>
+        <v>40496</v>
       </c>
       <c r="J20">
-        <v>301</v>
+        <v>39848</v>
       </c>
       <c r="K20">
-        <v>24</v>
+        <v>39198</v>
       </c>
       <c r="L20">
-        <v>545</v>
+        <v>38547</v>
       </c>
       <c r="M20">
-        <v>1863</v>
+        <v>37893</v>
       </c>
       <c r="N20">
-        <v>3977</v>
+        <v>37238</v>
       </c>
       <c r="O20">
-        <v>6886</v>
+        <v>36582</v>
       </c>
       <c r="P20">
-        <v>10587</v>
+        <v>35924</v>
       </c>
       <c r="Q20">
-        <v>15079</v>
+        <v>35265</v>
       </c>
       <c r="R20">
-        <v>20361</v>
+        <v>34606</v>
       </c>
       <c r="S20">
-        <v>26430</v>
+        <v>33945</v>
       </c>
       <c r="T20">
         <v>33284</v>
       </c>
       <c r="U20">
-        <v>40921</v>
+        <v>32623</v>
       </c>
       <c r="V20">
-        <v>49339</v>
+        <v>31961</v>
       </c>
       <c r="W20">
-        <v>58535</v>
+        <v>31299</v>
       </c>
       <c r="X20">
-        <v>68506</v>
+        <v>30637</v>
       </c>
       <c r="Y20">
-        <v>79251</v>
+        <v>29976</v>
       </c>
       <c r="Z20">
-        <v>90766</v>
+        <v>29315</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -1974,79 +1974,79 @@
         <v>3.56875</v>
       </c>
       <c r="B21">
-        <v>32099</v>
+        <v>53663</v>
       </c>
       <c r="C21">
-        <v>25320</v>
+        <v>52979</v>
       </c>
       <c r="D21">
-        <v>19344</v>
+        <v>52293</v>
       </c>
       <c r="E21">
-        <v>14173</v>
+        <v>51603</v>
       </c>
       <c r="F21">
-        <v>9807</v>
+        <v>50909</v>
       </c>
       <c r="G21">
-        <v>6243</v>
+        <v>50213</v>
       </c>
       <c r="H21">
-        <v>3483</v>
+        <v>49513</v>
       </c>
       <c r="I21">
-        <v>1525</v>
+        <v>48810</v>
       </c>
       <c r="J21">
-        <v>369</v>
+        <v>48105</v>
       </c>
       <c r="K21">
-        <v>13</v>
+        <v>47397</v>
       </c>
       <c r="L21">
-        <v>457</v>
+        <v>46686</v>
       </c>
       <c r="M21">
-        <v>1700</v>
+        <v>45973</v>
       </c>
       <c r="N21">
-        <v>3739</v>
+        <v>45257</v>
       </c>
       <c r="O21">
-        <v>6574</v>
+        <v>44539</v>
       </c>
       <c r="P21">
-        <v>10203</v>
+        <v>43819</v>
       </c>
       <c r="Q21">
-        <v>14624</v>
+        <v>43097</v>
       </c>
       <c r="R21">
-        <v>19836</v>
+        <v>42373</v>
       </c>
       <c r="S21">
-        <v>25836</v>
+        <v>41648</v>
       </c>
       <c r="T21">
-        <v>32623</v>
+        <v>40921</v>
       </c>
       <c r="U21">
         <v>40193</v>
       </c>
       <c r="V21">
-        <v>48545</v>
+        <v>39464</v>
       </c>
       <c r="W21">
-        <v>57677</v>
+        <v>38733</v>
       </c>
       <c r="X21">
-        <v>67585</v>
+        <v>38002</v>
       </c>
       <c r="Y21">
-        <v>78268</v>
+        <v>37271</v>
       </c>
       <c r="Z21">
-        <v>89722</v>
+        <v>36539</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -2054,79 +2054,79 @@
         <v>3.575</v>
       </c>
       <c r="B22">
-        <v>32853</v>
+        <v>63121</v>
       </c>
       <c r="C22">
-        <v>25984</v>
+        <v>62386</v>
       </c>
       <c r="D22">
-        <v>19921</v>
+        <v>61647</v>
       </c>
       <c r="E22">
-        <v>14664</v>
+        <v>60904</v>
       </c>
       <c r="F22">
-        <v>10212</v>
+        <v>60157</v>
       </c>
       <c r="G22">
-        <v>6565</v>
+        <v>59406</v>
       </c>
       <c r="H22">
-        <v>3722</v>
+        <v>58652</v>
       </c>
       <c r="I22">
-        <v>1682</v>
+        <v>57893</v>
       </c>
       <c r="J22">
-        <v>446</v>
+        <v>57132</v>
       </c>
       <c r="K22">
-        <v>11</v>
+        <v>56366</v>
       </c>
       <c r="L22">
-        <v>377</v>
+        <v>55597</v>
       </c>
       <c r="M22">
-        <v>1543</v>
+        <v>54825</v>
       </c>
       <c r="N22">
-        <v>3507</v>
+        <v>54050</v>
       </c>
       <c r="O22">
-        <v>6267</v>
+        <v>53271</v>
       </c>
       <c r="P22">
-        <v>9823</v>
+        <v>52490</v>
       </c>
       <c r="Q22">
-        <v>14172</v>
+        <v>51706</v>
       </c>
       <c r="R22">
-        <v>19313</v>
+        <v>50919</v>
       </c>
       <c r="S22">
-        <v>25243</v>
+        <v>50130</v>
       </c>
       <c r="T22">
-        <v>31961</v>
+        <v>49339</v>
       </c>
       <c r="U22">
-        <v>39464</v>
+        <v>48545</v>
       </c>
       <c r="V22">
         <v>47750</v>
       </c>
       <c r="W22">
-        <v>56816</v>
+        <v>46952</v>
       </c>
       <c r="X22">
-        <v>66660</v>
+        <v>46153</v>
       </c>
       <c r="Y22">
-        <v>77280</v>
+        <v>45353</v>
       </c>
       <c r="Z22">
-        <v>88672</v>
+        <v>44551</v>
       </c>
     </row>
     <row r="23" spans="1:26">
@@ -2134,79 +2134,79 @@
         <v>3.58125</v>
       </c>
       <c r="B23">
-        <v>33625</v>
+        <v>73339</v>
       </c>
       <c r="C23">
-        <v>26666</v>
+        <v>72554</v>
       </c>
       <c r="D23">
-        <v>20515</v>
+        <v>71764</v>
       </c>
       <c r="E23">
-        <v>15170</v>
+        <v>70969</v>
       </c>
       <c r="F23">
-        <v>10631</v>
+        <v>70169</v>
       </c>
       <c r="G23">
-        <v>6899</v>
+        <v>69365</v>
       </c>
       <c r="H23">
-        <v>3972</v>
+        <v>68556</v>
       </c>
       <c r="I23">
-        <v>1850</v>
+        <v>67743</v>
       </c>
       <c r="J23">
-        <v>532</v>
+        <v>66926</v>
       </c>
       <c r="K23">
-        <v>18</v>
+        <v>66104</v>
       </c>
       <c r="L23">
-        <v>305</v>
+        <v>65278</v>
       </c>
       <c r="M23">
-        <v>1392</v>
+        <v>64448</v>
       </c>
       <c r="N23">
-        <v>3280</v>
+        <v>63614</v>
       </c>
       <c r="O23">
-        <v>5965</v>
+        <v>62776</v>
       </c>
       <c r="P23">
-        <v>9446</v>
+        <v>61935</v>
       </c>
       <c r="Q23">
-        <v>13722</v>
+        <v>61090</v>
       </c>
       <c r="R23">
-        <v>18791</v>
+        <v>60241</v>
       </c>
       <c r="S23">
-        <v>24651</v>
+        <v>59390</v>
       </c>
       <c r="T23">
-        <v>31299</v>
+        <v>58535</v>
       </c>
       <c r="U23">
-        <v>38733</v>
+        <v>57677</v>
       </c>
       <c r="V23">
-        <v>46952</v>
+        <v>56816</v>
       </c>
       <c r="W23">
         <v>55953</v>
       </c>
       <c r="X23">
-        <v>65732</v>
+        <v>55087</v>
       </c>
       <c r="Y23">
-        <v>76288</v>
+        <v>54218</v>
       </c>
       <c r="Z23">
-        <v>87618</v>
+        <v>53348</v>
       </c>
     </row>
     <row r="24" spans="1:26">
@@ -2214,79 +2214,79 @@
         <v>3.5875</v>
       </c>
       <c r="B24">
-        <v>34415</v>
+        <v>84314</v>
       </c>
       <c r="C24">
-        <v>27366</v>
+        <v>83479</v>
       </c>
       <c r="D24">
-        <v>21124</v>
+        <v>82639</v>
       </c>
       <c r="E24">
-        <v>15691</v>
+        <v>81793</v>
       </c>
       <c r="F24">
-        <v>11065</v>
+        <v>80942</v>
       </c>
       <c r="G24">
-        <v>7247</v>
+        <v>80086</v>
       </c>
       <c r="H24">
-        <v>4235</v>
+        <v>79224</v>
       </c>
       <c r="I24">
-        <v>2029</v>
+        <v>78357</v>
       </c>
       <c r="J24">
-        <v>629</v>
+        <v>77485</v>
       </c>
       <c r="K24">
-        <v>33</v>
+        <v>76608</v>
       </c>
       <c r="L24">
-        <v>240</v>
+        <v>75726</v>
       </c>
       <c r="M24">
-        <v>1249</v>
+        <v>74839</v>
       </c>
       <c r="N24">
-        <v>3058</v>
+        <v>73948</v>
       </c>
       <c r="O24">
-        <v>5667</v>
+        <v>73052</v>
       </c>
       <c r="P24">
-        <v>9073</v>
+        <v>72151</v>
       </c>
       <c r="Q24">
-        <v>13275</v>
+        <v>71246</v>
       </c>
       <c r="R24">
-        <v>18271</v>
+        <v>70337</v>
       </c>
       <c r="S24">
-        <v>24059</v>
+        <v>69424</v>
       </c>
       <c r="T24">
-        <v>30637</v>
+        <v>68506</v>
       </c>
       <c r="U24">
-        <v>38002</v>
+        <v>67585</v>
       </c>
       <c r="V24">
-        <v>46153</v>
+        <v>66660</v>
       </c>
       <c r="W24">
-        <v>55087</v>
+        <v>65732</v>
       </c>
       <c r="X24">
         <v>64800</v>
       </c>
       <c r="Y24">
-        <v>75292</v>
+        <v>63865</v>
       </c>
       <c r="Z24">
-        <v>86558</v>
+        <v>62927</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -2294,79 +2294,79 @@
         <v>3.59375</v>
       </c>
       <c r="B25">
-        <v>35225</v>
+        <v>96044</v>
       </c>
       <c r="C25">
-        <v>28083</v>
+        <v>95161</v>
       </c>
       <c r="D25">
-        <v>21751</v>
+        <v>94271</v>
       </c>
       <c r="E25">
-        <v>16228</v>
+        <v>93375</v>
       </c>
       <c r="F25">
-        <v>11514</v>
+        <v>92473</v>
       </c>
       <c r="G25">
-        <v>7608</v>
+        <v>91565</v>
       </c>
       <c r="H25">
-        <v>4510</v>
+        <v>90652</v>
       </c>
       <c r="I25">
-        <v>2220</v>
+        <v>89732</v>
       </c>
       <c r="J25">
-        <v>736</v>
+        <v>88806</v>
       </c>
       <c r="K25">
-        <v>57</v>
+        <v>87875</v>
       </c>
       <c r="L25">
-        <v>183</v>
+        <v>86938</v>
       </c>
       <c r="M25">
-        <v>1112</v>
+        <v>85996</v>
       </c>
       <c r="N25">
-        <v>2843</v>
+        <v>85048</v>
       </c>
       <c r="O25">
-        <v>5375</v>
+        <v>84094</v>
       </c>
       <c r="P25">
-        <v>8705</v>
+        <v>83136</v>
       </c>
       <c r="Q25">
-        <v>12832</v>
+        <v>82172</v>
       </c>
       <c r="R25">
-        <v>17754</v>
+        <v>81203</v>
       </c>
       <c r="S25">
-        <v>23469</v>
+        <v>80230</v>
       </c>
       <c r="T25">
-        <v>29976</v>
+        <v>79251</v>
       </c>
       <c r="U25">
-        <v>37271</v>
+        <v>78268</v>
       </c>
       <c r="V25">
-        <v>45353</v>
+        <v>77280</v>
       </c>
       <c r="W25">
-        <v>54218</v>
+        <v>76288</v>
       </c>
       <c r="X25">
-        <v>63865</v>
+        <v>75292</v>
       </c>
       <c r="Y25">
         <v>74291</v>
       </c>
       <c r="Z25">
-        <v>85493</v>
+        <v>73287</v>
       </c>
     </row>
     <row r="26" spans="1:26">
@@ -2374,76 +2374,76 @@
         <v>3.6</v>
       </c>
       <c r="B26">
-        <v>36055</v>
+        <v>108526</v>
       </c>
       <c r="C26">
-        <v>28819</v>
+        <v>107595</v>
       </c>
       <c r="D26">
-        <v>22395</v>
+        <v>106657</v>
       </c>
       <c r="E26">
-        <v>16781</v>
+        <v>105712</v>
       </c>
       <c r="F26">
-        <v>11977</v>
+        <v>104760</v>
       </c>
       <c r="G26">
-        <v>7983</v>
+        <v>103802</v>
       </c>
       <c r="H26">
-        <v>4798</v>
+        <v>102837</v>
       </c>
       <c r="I26">
-        <v>2422</v>
+        <v>101866</v>
       </c>
       <c r="J26">
-        <v>853</v>
+        <v>100888</v>
       </c>
       <c r="K26">
-        <v>91</v>
+        <v>99903</v>
       </c>
       <c r="L26">
-        <v>135</v>
+        <v>98912</v>
       </c>
       <c r="M26">
-        <v>983</v>
+        <v>97915</v>
       </c>
       <c r="N26">
-        <v>2635</v>
+        <v>96912</v>
       </c>
       <c r="O26">
-        <v>5088</v>
+        <v>95902</v>
       </c>
       <c r="P26">
-        <v>8341</v>
+        <v>94887</v>
       </c>
       <c r="Q26">
-        <v>12392</v>
+        <v>93865</v>
       </c>
       <c r="R26">
-        <v>17239</v>
+        <v>92838</v>
       </c>
       <c r="S26">
-        <v>22881</v>
+        <v>91805</v>
       </c>
       <c r="T26">
-        <v>29315</v>
+        <v>90766</v>
       </c>
       <c r="U26">
-        <v>36539</v>
+        <v>89722</v>
       </c>
       <c r="V26">
-        <v>44551</v>
+        <v>88672</v>
       </c>
       <c r="W26">
-        <v>53348</v>
+        <v>87618</v>
       </c>
       <c r="X26">
-        <v>62927</v>
+        <v>86558</v>
       </c>
       <c r="Y26">
-        <v>73287</v>
+        <v>85493</v>
       </c>
       <c r="Z26">
         <v>84423</v>

</xml_diff>